<commit_message>
HPCC-9999 from managed 20210525
Signed-off-by: KevinWang <kevin.wang@lexisnexis.com>
</commit_message>
<xml_diff>
--- a/esp/kw/notes/My Open Issues 001 (HPCC).xlsx
+++ b/esp/kw/notes/My Open Issues 001 (HPCC).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://reedelsevier-my.sharepoint.com/personal/wangkx_risk_regn_net/Documents/Desktop/notes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangkx\src\HPCC-Platform\esp\kw\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{1FD48228-7243-42DA-8AE0-C1C977C3F572}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3C5DE59E-D01C-48CC-983B-A8F7E5CF2EA6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8379275-5DDA-4FA9-903D-0AB28F93AC21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="My Open Issues 001 (HPCC) 2020-" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="298">
   <si>
     <t>all</t>
   </si>
@@ -616,9 +616,6 @@
     <t>Physical Memory Data is nested inside of storage data response for preflight pages</t>
   </si>
   <si>
-    <t>Security hole submitting a workunit</t>
-  </si>
-  <si>
     <t>Exclude Indexes from file list</t>
   </si>
   <si>
@@ -736,9 +733,6 @@
     <t>Rodrigo?</t>
   </si>
   <si>
-    <t>g1</t>
-  </si>
-  <si>
     <t>Why takes a long time to read Wus from dfuserver queue.</t>
   </si>
   <si>
@@ -775,16 +769,163 @@
     <t>Tony? Wait?</t>
   </si>
   <si>
-    <t>Part size, etc</t>
-  </si>
-  <si>
-    <t>Reject FileAccess2 if missing/invalid keys</t>
+    <t>ldap</t>
   </si>
   <si>
     <t>unused file for dfuxref</t>
   </si>
   <si>
-    <t>ldap</t>
+    <t>DFUXref</t>
+  </si>
+  <si>
+    <t>compressed sizes</t>
+  </si>
+  <si>
+    <t>file size parrent</t>
+  </si>
+  <si>
+    <t>invalid LZ</t>
+  </si>
+  <si>
+    <t>part sizes</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>mysql logging</t>
+  </si>
+  <si>
+    <t>FileAccess2</t>
+  </si>
+  <si>
+    <t>WsDali</t>
+  </si>
+  <si>
+    <t>cluster display</t>
+  </si>
+  <si>
+    <t>Streaming Ptree</t>
+  </si>
+  <si>
+    <t>Remove eclcc from activity page</t>
+  </si>
+  <si>
+    <t>Slow for dfuserver when activity</t>
+  </si>
+  <si>
+    <t>WsDFUXref soapcall</t>
+  </si>
+  <si>
+    <t>ldap user token for cloud</t>
+  </si>
+  <si>
+    <t>cloud</t>
+  </si>
+  <si>
+    <t>mn</t>
+  </si>
+  <si>
+    <t>Too many WUs in queues</t>
+  </si>
+  <si>
+    <t>permission errors</t>
+  </si>
+  <si>
+    <t>not in env?</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Disk Usage on swap node</t>
+  </si>
+  <si>
+    <t>TpWrapper</t>
+  </si>
+  <si>
+    <t>ws_fsbinding</t>
+  </si>
+  <si>
+    <t>ws_dfuservice  cloud environment</t>
+  </si>
+  <si>
+    <t>ws_dfuxrefservice  cloud environment</t>
+  </si>
+  <si>
+    <t>ws_fs</t>
+  </si>
+  <si>
+    <t>ws_machine</t>
+  </si>
+  <si>
+    <t>ws_topology</t>
+  </si>
+  <si>
+    <t>Ws_package</t>
+  </si>
+  <si>
+    <t>orig</t>
+  </si>
+  <si>
+    <t>combine ESPenum 3 options</t>
+  </si>
+  <si>
+    <t>FileIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>sasha in wu service</t>
+  </si>
+  <si>
+    <t>ESP memory</t>
+  </si>
+  <si>
+    <t>Base on Gavin's PR?</t>
+  </si>
+  <si>
+    <t>in wsdfu</t>
+  </si>
+  <si>
+    <t>Ws_workunitH</t>
+  </si>
+  <si>
+    <t>Ws_workunitS</t>
+  </si>
+  <si>
+    <t>Ws_workunitQ</t>
+  </si>
+  <si>
+    <t>Fixed in 25837</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>in 25842</t>
+  </si>
+  <si>
+    <t>Jake?how to check http or https</t>
+  </si>
+  <si>
+    <t>TPWrap</t>
+  </si>
+  <si>
+    <t>after 25833</t>
+  </si>
+  <si>
+    <t>after 25833, add throw exception in DFUWUSearch for cloud</t>
   </si>
 </sst>
 </file>
@@ -953,7 +1094,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1141,13 +1282,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1312,7 +1459,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1334,7 +1481,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1690,10 +1842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R150"/>
+  <dimension ref="A1:R155"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="A145" sqref="A145:XFD145"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130:C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2850,10 +3002,10 @@
         <v>31</v>
       </c>
       <c r="C81" t="s">
+        <v>221</v>
+      </c>
+      <c r="D81" t="s">
         <v>222</v>
-      </c>
-      <c r="D81" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -3105,7 +3257,7 @@
         <v>31</v>
       </c>
       <c r="C99" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -3113,7 +3265,7 @@
         <v>23524</v>
       </c>
       <c r="C100" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D100" t="s">
         <v>38</v>
@@ -3127,7 +3279,7 @@
         <v>31</v>
       </c>
       <c r="C101" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -3138,7 +3290,7 @@
         <v>31</v>
       </c>
       <c r="C102" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -3163,7 +3315,7 @@
         <v>31</v>
       </c>
       <c r="C104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3202,7 +3354,7 @@
         <v>96</v>
       </c>
       <c r="C107" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -3288,7 +3440,7 @@
         <v>31</v>
       </c>
       <c r="C114" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3299,7 +3451,7 @@
         <v>96</v>
       </c>
       <c r="C115" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3379,10 +3531,10 @@
         <v>24835</v>
       </c>
       <c r="C122" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E122" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -3390,10 +3542,10 @@
         <v>24848</v>
       </c>
       <c r="C123" t="s">
+        <v>208</v>
+      </c>
+      <c r="E123" t="s">
         <v>209</v>
-      </c>
-      <c r="E123" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -3409,7 +3561,7 @@
         <v>31</v>
       </c>
       <c r="C125" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -3425,10 +3577,10 @@
         <v>31</v>
       </c>
       <c r="C127" t="s">
+        <v>205</v>
+      </c>
+      <c r="D127" t="s">
         <v>206</v>
-      </c>
-      <c r="D127" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -3497,10 +3649,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>25071</v>
+        <v>25085</v>
       </c>
       <c r="B133" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="C133" t="s">
         <v>194</v>
@@ -3508,7 +3660,7 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>25085</v>
+        <v>25092</v>
       </c>
       <c r="B134" t="s">
         <v>96</v>
@@ -3519,10 +3671,10 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>25092</v>
+        <v>25168</v>
       </c>
       <c r="B135" t="s">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="C135" t="s">
         <v>196</v>
@@ -3530,31 +3682,31 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>25168</v>
+        <v>25172</v>
       </c>
       <c r="B136" t="s">
         <v>31</v>
       </c>
       <c r="C136" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>25172</v>
+        <v>25217</v>
       </c>
       <c r="B137" t="s">
         <v>31</v>
       </c>
       <c r="C137" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>25217</v>
-      </c>
-      <c r="B138" t="s">
+        <v>25218</v>
+      </c>
+      <c r="B138" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C138" t="s">
@@ -3563,9 +3715,9 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>25218</v>
-      </c>
-      <c r="B139" s="8" t="s">
+        <v>25229</v>
+      </c>
+      <c r="B139" t="s">
         <v>31</v>
       </c>
       <c r="C139" t="s">
@@ -3574,69 +3726,145 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>25229</v>
-      </c>
-      <c r="B140" t="s">
-        <v>31</v>
+        <v>25230</v>
       </c>
       <c r="C140" t="s">
-        <v>203</v>
+        <v>262</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>25230</v>
+        <v>25236</v>
+      </c>
+      <c r="C141" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>25236</v>
+        <v>25279</v>
+      </c>
+      <c r="B142" t="s">
+        <v>31</v>
+      </c>
+      <c r="C142" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>25279</v>
-      </c>
-      <c r="B143" t="s">
-        <v>31</v>
+        <v>25387</v>
       </c>
       <c r="C143" t="s">
-        <v>205</v>
+        <v>260</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>25327</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+        <v>25389</v>
+      </c>
+      <c r="C144" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>25387</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+        <v>25391</v>
+      </c>
+      <c r="C145" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>25389</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+        <v>25419</v>
+      </c>
+      <c r="C146" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>25391</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+        <v>25447</v>
+      </c>
+      <c r="B147" t="s">
+        <v>252</v>
+      </c>
+      <c r="C147" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>25419</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+        <v>25498</v>
+      </c>
+      <c r="C148" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>25444</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+        <v>25520</v>
+      </c>
+      <c r="B149" t="s">
+        <v>253</v>
+      </c>
+      <c r="C149" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>25447</v>
+        <v>25522</v>
+      </c>
+      <c r="C150" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>25540</v>
+      </c>
+      <c r="C151" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>25554</v>
+      </c>
+      <c r="B152" t="s">
+        <v>252</v>
+      </c>
+      <c r="C152" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>25556</v>
+      </c>
+      <c r="B153" t="s">
+        <v>253</v>
+      </c>
+      <c r="C153" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>25622</v>
+      </c>
+      <c r="C154" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>25684</v>
+      </c>
+      <c r="C155" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -3649,10 +3877,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E85888-7E64-4969-8811-D623AAAF1A88}">
-  <dimension ref="A1:M55"/>
+  <dimension ref="A1:X76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3686,763 +3914,1112 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
-        <v>25684</v>
-      </c>
-      <c r="B4" s="10">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>25622</v>
-      </c>
-      <c r="B5" s="2">
+    <row r="3" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14">
+        <v>24953</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14">
+        <v>25860</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>25855</v>
+      </c>
+      <c r="B8" s="14">
         <v>2</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
-        <v>25522</v>
-      </c>
-      <c r="B6" s="10">
-        <v>2</v>
-      </c>
-      <c r="C6" s="10">
-        <v>2</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>25498</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>25419</v>
-      </c>
-      <c r="E8" t="s">
-        <v>238</v>
-      </c>
-      <c r="M8" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>25391</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>236</v>
+      <c r="E8" s="14" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14">
+        <v>25843</v>
+      </c>
+      <c r="B9" s="14">
+        <v>0</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
+        <v>25842</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>25841</v>
+      </c>
+      <c r="B11" s="16">
+        <v>1</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>25840</v>
+      </c>
+      <c r="B12" s="16">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>25839</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14">
+        <v>25838</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14">
+        <v>25836</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
+        <v>25835</v>
+      </c>
+      <c r="B16" s="16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>25834</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
+        <v>25833</v>
+      </c>
+      <c r="B18" s="16">
+        <v>1</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>25832</v>
+      </c>
+      <c r="B19" s="1">
+        <v>4</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="M19" s="10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>25820</v>
+      </c>
+      <c r="B20" s="1">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="M20" s="10" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>25819</v>
+      </c>
+      <c r="B21" s="1">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="M21" s="10" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
+        <v>25817</v>
+      </c>
+      <c r="B22" s="16">
+        <v>1</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14">
+        <v>25770</v>
+      </c>
+      <c r="B23" s="14">
+        <v>2</v>
+      </c>
+      <c r="C23" s="14">
+        <v>2</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
+        <v>25742</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A25" s="12">
+        <v>25622</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="M25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <v>25540</v>
+      </c>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="M26" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25419</v>
+      </c>
+      <c r="E27" t="s">
+        <v>236</v>
+      </c>
+      <c r="M27" t="s">
+        <v>237</v>
+      </c>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13"/>
+      <c r="W27" s="13"/>
+    </row>
+    <row r="28" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>25391</v>
+      </c>
+      <c r="B28" s="1">
+        <v>9</v>
+      </c>
+      <c r="C28" s="1">
+        <v>3</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="U28" s="13"/>
+      <c r="V28" s="13"/>
+      <c r="W28" s="13"/>
+      <c r="X28"/>
+    </row>
+    <row r="29" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>25389</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B29" s="1">
+        <v>5</v>
+      </c>
+      <c r="C29" s="1">
         <v>2</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D29" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="U29" s="13"/>
+      <c r="V29" s="13"/>
+      <c r="W29" s="13"/>
+      <c r="X29"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>25387</v>
+      </c>
+      <c r="E30" t="s">
+        <v>233</v>
+      </c>
+      <c r="M30" t="s">
+        <v>265</v>
+      </c>
+      <c r="U30" s="13"/>
+      <c r="V30" s="13"/>
+      <c r="W30" s="13"/>
+    </row>
+    <row r="31" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
+        <v>25279</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="M31" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>25236</v>
+      </c>
+      <c r="B32" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" t="s">
+        <v>241</v>
+      </c>
+      <c r="M32" t="s">
+        <v>242</v>
+      </c>
+      <c r="U32" s="13"/>
+      <c r="V32" s="13"/>
+      <c r="W32" s="13"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>25230</v>
+      </c>
+      <c r="B33" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" t="s">
+        <v>243</v>
+      </c>
+      <c r="M33" t="s">
+        <v>244</v>
+      </c>
+      <c r="U33" s="13"/>
+      <c r="V33" s="13"/>
+      <c r="W33" s="13"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>25229</v>
+      </c>
+      <c r="E34" t="s">
+        <v>202</v>
+      </c>
+      <c r="M34" t="s">
+        <v>203</v>
+      </c>
+      <c r="U34" s="13"/>
+      <c r="V34" s="13"/>
+      <c r="W34" s="13"/>
+    </row>
+    <row r="35" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13">
+        <v>25218</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="M35" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13">
+        <v>25217</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="M36" s="13" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13">
+        <v>25172</v>
+      </c>
+      <c r="B37" s="13">
+        <v>3</v>
+      </c>
+      <c r="C37" s="13">
         <v>2</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E37" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="M37" s="13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13">
+        <v>25168</v>
+      </c>
+      <c r="B38" s="13">
+        <v>9</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13">
+        <v>25085</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13">
+        <v>25042</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13">
+        <v>25025</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="U41" s="13"/>
+      <c r="V41" s="13"/>
+      <c r="W41" s="13"/>
+      <c r="X41"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>25010</v>
+      </c>
+      <c r="B42" s="1">
+        <v>4</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="U42" s="13"/>
+      <c r="V42" s="13"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>24968</v>
+      </c>
+      <c r="E43" t="s">
+        <v>184</v>
+      </c>
+      <c r="U43" s="13"/>
+      <c r="V43" s="13"/>
+    </row>
+    <row r="44" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>24917</v>
+      </c>
+      <c r="B44" s="2">
+        <v>5</v>
+      </c>
+      <c r="C44" s="2">
+        <v>2</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="U44" s="13"/>
+      <c r="V44" s="13"/>
+      <c r="X44"/>
+    </row>
+    <row r="45" spans="1:24" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="10">
+        <v>24895</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="M45" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="U45" s="13"/>
+      <c r="V45" s="13"/>
+      <c r="W45" s="13"/>
+      <c r="X45"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>24710</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>25387</v>
-      </c>
-      <c r="C11">
+      <c r="E46" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+    </row>
+    <row r="47" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>24652</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="X47"/>
+    </row>
+    <row r="48" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>24496</v>
+      </c>
+      <c r="C48" s="2">
+        <v>3</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="M48" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="X48"/>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>24412</v>
+      </c>
+      <c r="B49" s="1">
+        <v>6</v>
+      </c>
+      <c r="C49" s="1">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>25643</v>
-      </c>
-      <c r="B12" s="1">
+      <c r="D49" s="1"/>
+      <c r="E49" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
+        <v>24303</v>
+      </c>
+      <c r="B50" s="5">
+        <v>7</v>
+      </c>
+      <c r="C50" s="5">
         <v>2</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D50" s="2"/>
+      <c r="E50" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+    </row>
+    <row r="51" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>24156</v>
+      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="5">
+        <v>3</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="X51"/>
+    </row>
+    <row r="52" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>23990</v>
+      </c>
+      <c r="B52" s="4"/>
+      <c r="C52" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="D52"/>
+      <c r="E52" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+      <c r="V52" s="13"/>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>23811</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="3"/>
+      <c r="E53" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="M53" t="s">
+        <v>203</v>
+      </c>
+      <c r="V53" s="13"/>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>23494</v>
+      </c>
+      <c r="B54" s="4"/>
+      <c r="C54" s="3">
+        <v>3</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="V54" s="13"/>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>22056</v>
+      </c>
+      <c r="B55" s="4"/>
+      <c r="C55" s="3"/>
+      <c r="E55" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="M55" t="s">
+        <v>240</v>
+      </c>
+      <c r="V55" s="13"/>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>21500</v>
+      </c>
+      <c r="B56" s="4"/>
+      <c r="C56" s="3">
         <v>2</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>158</v>
-      </c>
-      <c r="E13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>25236</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D56" t="s">
         <v>146</v>
       </c>
-      <c r="E15" t="s">
-        <v>243</v>
-      </c>
-      <c r="M15" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>25230</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="E56" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M56" t="s">
+        <v>149</v>
+      </c>
+      <c r="V56" s="13"/>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>21140</v>
+      </c>
+      <c r="B57" s="4"/>
+      <c r="C57" s="3">
+        <v>2</v>
+      </c>
+      <c r="D57" t="s">
         <v>146</v>
       </c>
-      <c r="E16" t="s">
-        <v>245</v>
-      </c>
-      <c r="M16" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>25229</v>
-      </c>
-      <c r="C17">
+      <c r="E57" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="M57" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>21067</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+      <c r="E58" t="s">
+        <v>108</v>
+      </c>
+      <c r="M58" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>20967</v>
+      </c>
+      <c r="B59" s="4"/>
+      <c r="C59" s="3">
+        <v>3</v>
+      </c>
+      <c r="D59" t="s">
+        <v>146</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="M59" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>20908</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="E60" t="s">
+        <v>109</v>
+      </c>
+      <c r="M60" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>20697</v>
+      </c>
+      <c r="B61" s="4"/>
+      <c r="C61" s="3">
+        <v>3</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>20022</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+      <c r="D62" t="s">
+        <v>146</v>
+      </c>
+      <c r="E62" t="s">
+        <v>71</v>
+      </c>
+      <c r="M62" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>20021</v>
+      </c>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2">
+        <v>3</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+      <c r="M63" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A64" s="6">
+        <v>19461</v>
+      </c>
+      <c r="B64" s="6"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+      <c r="I64" s="2"/>
+      <c r="J64" s="2"/>
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+      <c r="M64" s="2"/>
+    </row>
+    <row r="65" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>19460</v>
+      </c>
+      <c r="B65" s="4"/>
+      <c r="C65" s="3"/>
+      <c r="D65"/>
+      <c r="E65" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F65"/>
+      <c r="G65"/>
+      <c r="H65"/>
+      <c r="I65"/>
+      <c r="J65"/>
+      <c r="K65"/>
+      <c r="L65"/>
+      <c r="M65"/>
+    </row>
+    <row r="66" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>19279</v>
+      </c>
+      <c r="B66" s="4"/>
+      <c r="C66" s="3">
+        <v>3</v>
+      </c>
+      <c r="D66"/>
+      <c r="E66" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F66"/>
+      <c r="G66"/>
+      <c r="H66"/>
+      <c r="I66"/>
+      <c r="J66"/>
+      <c r="K66"/>
+      <c r="L66"/>
+      <c r="M66" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>19278</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+      <c r="E67" t="s">
+        <v>138</v>
+      </c>
+      <c r="M67" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>19276</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
+      </c>
+      <c r="E68" t="s">
+        <v>83</v>
+      </c>
+      <c r="M68" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>17921</v>
+      </c>
+      <c r="C69">
+        <v>3</v>
+      </c>
+      <c r="E69" t="s">
+        <v>86</v>
+      </c>
+      <c r="M69" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>16718</v>
+      </c>
+      <c r="B70" s="4"/>
+      <c r="C70" s="3">
+        <v>3</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="M70" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>178</v>
+      </c>
+      <c r="E72" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1">
         <v>2</v>
       </c>
-      <c r="E17" t="s">
-        <v>203</v>
-      </c>
-      <c r="M17" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>25092</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>25010</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>24968</v>
-      </c>
-      <c r="E20" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>24917</v>
-      </c>
-      <c r="B21" s="2">
-        <v>5</v>
-      </c>
-      <c r="C21" s="2">
-        <v>2</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
-        <v>24895</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="D22" s="11" t="s">
+      <c r="D73" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="M22" s="11" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>24710</v>
-      </c>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1">
-        <v>2</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>24652</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>24496</v>
-      </c>
-      <c r="C25" s="2">
-        <v>3</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>24412</v>
-      </c>
-      <c r="B26" s="1">
-        <v>6</v>
-      </c>
-      <c r="C26" s="1">
-        <v>2</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
-        <v>24303</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5">
-        <v>2</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-    </row>
-    <row r="28" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
-        <v>24156</v>
-      </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="5">
-        <v>3</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
-        <v>23990</v>
-      </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="3">
-        <v>2</v>
-      </c>
-      <c r="D29"/>
-      <c r="E29" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="F29"/>
-      <c r="G29"/>
-      <c r="H29"/>
-      <c r="I29"/>
-      <c r="J29"/>
-      <c r="K29"/>
-      <c r="L29"/>
-      <c r="M29"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
-        <v>23811</v>
-      </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="3"/>
-      <c r="E30" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="M30" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
-        <v>23634</v>
-      </c>
-      <c r="B31" s="4">
-        <v>5</v>
-      </c>
-      <c r="C31" s="3">
-        <v>2</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
-        <v>23494</v>
-      </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="3">
-        <v>3</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
-        <v>22056</v>
-      </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="3"/>
-      <c r="E33" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="M33" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
-        <v>21500</v>
-      </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="3">
-        <v>2</v>
-      </c>
-      <c r="D34" t="s">
-        <v>146</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="M34" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>21140</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="3">
-        <v>2</v>
-      </c>
-      <c r="D35" t="s">
-        <v>146</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="M35" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>21067</v>
-      </c>
-      <c r="C36">
-        <v>3</v>
-      </c>
-      <c r="E36" t="s">
-        <v>108</v>
-      </c>
-      <c r="M36" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <v>20967</v>
-      </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="3">
-        <v>3</v>
-      </c>
-      <c r="D37" t="s">
-        <v>146</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="M37" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>20908</v>
-      </c>
-      <c r="C38">
-        <v>3</v>
-      </c>
-      <c r="E38" t="s">
-        <v>109</v>
-      </c>
-      <c r="M38" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <v>20697</v>
-      </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="3">
-        <v>3</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>20022</v>
-      </c>
-      <c r="C40">
-        <v>3</v>
-      </c>
-      <c r="D40" t="s">
-        <v>146</v>
-      </c>
-      <c r="E40" t="s">
-        <v>71</v>
-      </c>
-      <c r="M40" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
-        <v>20021</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2">
-        <v>3</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="6">
-        <v>19461</v>
-      </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="5">
-        <v>3</v>
-      </c>
-      <c r="D42" s="2"/>
-      <c r="E42" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-    </row>
-    <row r="43" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
-        <v>19460</v>
-      </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="3">
-        <v>3</v>
-      </c>
-      <c r="D43"/>
-      <c r="E43" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F43"/>
-      <c r="G43"/>
-      <c r="H43"/>
-      <c r="I43"/>
-      <c r="J43"/>
-      <c r="K43"/>
-      <c r="L43"/>
-      <c r="M43"/>
-    </row>
-    <row r="44" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
-        <v>19279</v>
-      </c>
-      <c r="B44" s="4"/>
-      <c r="C44" s="3">
-        <v>3</v>
-      </c>
-      <c r="D44"/>
-      <c r="E44" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F44"/>
-      <c r="G44"/>
-      <c r="H44"/>
-      <c r="I44"/>
-      <c r="J44"/>
-      <c r="K44"/>
-      <c r="L44"/>
-      <c r="M44" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>19278</v>
-      </c>
-      <c r="C45">
-        <v>3</v>
-      </c>
-      <c r="E45" t="s">
-        <v>138</v>
-      </c>
-      <c r="M45" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>19276</v>
-      </c>
-      <c r="C46">
-        <v>3</v>
-      </c>
-      <c r="E46" t="s">
-        <v>83</v>
-      </c>
-      <c r="M46" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>17921</v>
-      </c>
-      <c r="C47">
-        <v>3</v>
-      </c>
-      <c r="E47" t="s">
-        <v>86</v>
-      </c>
-      <c r="M47" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
-        <v>17334</v>
-      </c>
-      <c r="B48" s="4"/>
-      <c r="C48" s="3">
-        <v>3</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
-        <v>16718</v>
-      </c>
-      <c r="B49" s="4"/>
-      <c r="C49" s="3">
-        <v>3</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="M49" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E50" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
-        <v>178</v>
-      </c>
-      <c r="E51" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1">
-        <v>2</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E52" s="1" t="s">
+      <c r="E73" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2" t="s">
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E55" s="4"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+      <c r="M74" s="2"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E76" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:M51">
-    <sortCondition descending="1" ref="A17:A51"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="U25:W51">
+    <sortCondition descending="1" ref="U25:U51"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4474,10 +5051,10 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4488,10 +5065,10 @@
         <v>31</v>
       </c>
       <c r="C4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" t="s">
         <v>203</v>
-      </c>
-      <c r="D4" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4502,10 +5079,10 @@
         <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4516,10 +5093,10 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4530,10 +5107,10 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
+        <v>198</v>
+      </c>
+      <c r="D7" t="s">
         <v>199</v>
-      </c>
-      <c r="D7" t="s">
-        <v>200</v>
       </c>
       <c r="H7" s="9"/>
     </row>
@@ -4545,10 +5122,10 @@
         <v>31</v>
       </c>
       <c r="C8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" t="s">
         <v>197</v>
-      </c>
-      <c r="D8" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4574,48 +5151,48 @@
         <v>96</v>
       </c>
       <c r="C10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" t="s">
         <v>215</v>
-      </c>
-      <c r="D10" t="s">
-        <v>216</v>
       </c>
       <c r="H10" s="9"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
+        <v>231</v>
+      </c>
+      <c r="D12" t="s">
         <v>232</v>
-      </c>
-      <c r="D12" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D16" t="s">
         <v>146</v>
@@ -4623,7 +5200,7 @@
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D17" t="s">
         <v>146</v>
@@ -4631,10 +5208,10 @@
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>